<commit_message>
Upload file via API
</commit_message>
<xml_diff>
--- a/gold calculator.xlsx
+++ b/gold calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s431328\OneDrive - Emirates Group\Desktop\Wissam\travian\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\travian\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B4171C-D106-4ECF-AC96-F1C8E3BB61B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098FCAAC-FC2A-4E75-A62C-5046D997C165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="93">
   <si>
     <t>wood</t>
   </si>
@@ -304,6 +304,21 @@
   <si>
     <t>alpha</t>
   </si>
+  <si>
+    <t>Hero inventory transfer amounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                           </t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>current hero inventory</t>
+  </si>
 </sst>
 </file>
 
@@ -350,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -408,8 +424,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0E845ED-06E6-4F8A-9AB4-3E1C46E9BA7B}" name="Table2" displayName="Table2" ref="G2:M7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="G2:M7" xr:uid="{D0E845ED-06E6-4F8A-9AB4-3E1C46E9BA7B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0E845ED-06E6-4F8A-9AB4-3E1C46E9BA7B}" name="Table2" displayName="Table2" ref="G2:M15" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="G2:M15" xr:uid="{D0E845ED-06E6-4F8A-9AB4-3E1C46E9BA7B}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{49693833-23A2-4F3C-8873-E73E5C19B51D}" name="item" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{C3124991-9E59-4B39-B699-AC5CB73A0A81}" name="level" dataDxfId="5"/>
@@ -694,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +723,7 @@
     <col min="9" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -723,8 +739,23 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -758,257 +789,687 @@
       <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="T2">
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>7311</v>
+        <v>500</v>
       </c>
       <c r="B3">
-        <v>931</v>
+        <v>730</v>
       </c>
       <c r="C3">
-        <v>7615</v>
+        <v>374</v>
       </c>
       <c r="D3">
-        <v>59237</v>
+        <v>19069</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>8800</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>11200</v>
+        <v>0</v>
       </c>
       <c r="K3" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>8400</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>7800</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>81</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>10105</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>8080</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>3030</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>6060</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>82</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>4</v>
+      </c>
+      <c r="U4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>2520</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>2310</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>1960</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>84</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>1560</v>
+        <v>0</v>
       </c>
       <c r="K6" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>660</v>
+        <v>0</v>
       </c>
       <c r="L6" s="1">
         <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>85</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="T6">
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>86</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="I8" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>MAX(A18-A3,0)</f>
+        <v>5440</v>
+      </c>
+      <c r="B9">
+        <f>MAX(B18-B3,0)</f>
+        <v>6470</v>
+      </c>
+      <c r="C9">
+        <f>MAX(C18-C3,0)</f>
+        <v>4616</v>
+      </c>
+      <c r="D9">
+        <f>MAX(D18-D3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>SUM(A9:D9)</f>
+        <v>16526</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="1">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>91</v>
+      </c>
+      <c r="R9">
+        <f>SUM(R2:R7)</f>
+        <v>24</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ref="S9:T9" si="0">SUM(S2:S7)</f>
+        <v>23</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="G12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="1">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>1980</v>
+      </c>
+      <c r="J13" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>2475</v>
+      </c>
+      <c r="K13" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>1735</v>
+      </c>
+      <c r="L13" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>495</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>135</v>
+      </c>
+      <c r="B14">
+        <v>117</v>
+      </c>
+      <c r="C14">
+        <v>183</v>
+      </c>
+      <c r="D14">
+        <v>313</v>
+      </c>
+      <c r="E14">
+        <f>SUM((A14:D14))*1000</f>
+        <v>748000</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="1">
         <v>15</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="I14" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>2535</v>
+      </c>
+      <c r="J14" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>3170</v>
+      </c>
+      <c r="K14" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>2220</v>
+      </c>
+      <c r="L14" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>635</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,4,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>1425</v>
+      </c>
+      <c r="J15" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,5,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>1555</v>
+      </c>
+      <c r="K15" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,6,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>1035</v>
+      </c>
+      <c r="L15" s="1">
+        <f>VLOOKUP(Table2[[#This Row],[item]]&amp;Table2[[#This Row],[level]],Sheet2!$A:$G,7,FALSE) * Table2[[#This Row],[count]]</f>
+        <v>160</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="R17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
         <f>SUM(I:I)</f>
-        <v>22625</v>
-      </c>
-      <c r="B15">
+        <v>5940</v>
+      </c>
+      <c r="B18">
         <f>SUM(J:J)</f>
-        <v>23150</v>
-      </c>
-      <c r="C15">
+        <v>7200</v>
+      </c>
+      <c r="C18">
         <f>SUM(K:K)</f>
-        <v>14050</v>
-      </c>
-      <c r="D15">
+        <v>4990</v>
+      </c>
+      <c r="D18">
         <f>SUM(L:L)</f>
-        <v>15060</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="4">
-        <f>SUM(A15:D15)</f>
-        <v>74885</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B22" s="4">
+        <f>SUM(A18:D18)</f>
+        <v>19420</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4">
-        <f>SUM(A3:D3) - SUM(A15:D15)</f>
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B23" s="4">
+        <f>SUM(A3:D3) - SUM(A18:D18)</f>
+        <v>1253</v>
+      </c>
+      <c r="C23" s="6">
+        <f>MAX(0,B23)</f>
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>83</v>
       </c>
-      <c r="B21">
-        <f>SUM(B24:B31)*B23</f>
+      <c r="B24">
+        <f>SUM(B27:B34)*B26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>80</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25">
-        <v>24960</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>84</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B27">
-        <v>12480</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24960</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
     </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30">
+        <v>12480</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="G1:M1"/>
-    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;K737373 BUSINESS DOCUMENT  This document is intended for business use and should be distributed to intended recipients only.</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -23028,6 +23489,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;K737373 BUSINESS DOCUMENT  This document is intended for business use and should be distributed to intended recipients only.</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -23328,6 +23792,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;K737373 BUSINESS DOCUMENT  This document is intended for business use and should be distributed to intended recipients only.</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -23635,5 +24102,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;K737373 BUSINESS DOCUMENT  This document is intended for business use and should be distributed to intended recipients only.</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>